<commit_message>
PAT code for facebook and matrix
</commit_message>
<xml_diff>
--- a/Dropbox/dropbox_mat.xlsx
+++ b/Dropbox/dropbox_mat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -439,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>7.1999999999999995E-2</v>
+        <v>10</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -596,79 +596,79 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.432</v>
+        <v>60</v>
       </c>
       <c r="I8">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" t="s">
-        <v>7</v>
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -697,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -729,10 +729,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -761,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -801,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -820,7 +820,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -841,68 +841,10 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0.86</v>
       </c>
       <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0.86</v>
-      </c>
-      <c r="I22">
         <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>